<commit_message>
adding csv to so
</commit_message>
<xml_diff>
--- a/Assets/Assets/Doc/ItemDatabase.xlsx
+++ b/Assets/Assets/Doc/ItemDatabase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeGame\Project\Knight\Assets\Assets\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D3054D5-2A73-4E6B-88CB-EFCDFD60FEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A478431B-46FF-41AE-86F8-66833A1203B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E0A02FB-42A1-4C3A-BAFD-43FAEF0C3AFD}"/>
   </bookViews>
@@ -36,22 +36,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Soul</t>
   </si>
   <si>
     <t>Currency for buying and trading item</t>
+  </si>
+  <si>
+    <t>Moonstone</t>
+  </si>
+  <si>
+    <t>Material for upgrading weapon</t>
+  </si>
+  <si>
+    <t>Plastic Flower</t>
+  </si>
+  <si>
+    <t>Delicacy flower, a gift which have not been given</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +95,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,18 +420,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BCC001-5419-42A3-8862-EE151A658C0E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -420,108 +443,41 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:3" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>